<commit_message>
#Manual de Instalacion OK #Instalador OK #Fix Rutas Plantillas OK #Casos de Prueba Descripcion en Carpeta OK
</commit_message>
<xml_diff>
--- a/Anotaciones/Plantilla Seguimiento TP-Plan Entrega.xlsx
+++ b/Anotaciones/Plantilla Seguimiento TP-Plan Entrega.xlsx
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +843,7 @@
         <v>48</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="2:7" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -857,7 +857,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:7" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
#Diagrama de Clases Entidades OK #DER OK #Limpieza de clases en codigo (ej: Politica y Limite)
</commit_message>
<xml_diff>
--- a/Anotaciones/Plantilla Seguimiento TP-Plan Entrega.xlsx
+++ b/Anotaciones/Plantilla Seguimiento TP-Plan Entrega.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>Tema</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>Q significa. Diagrama por cada Capa</t>
-  </si>
-  <si>
-    <t>Hacer</t>
   </si>
   <si>
     <t>OK</t>
@@ -640,7 +637,7 @@
   <dimension ref="B2:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +840,7 @@
         <v>48</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="2:7" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -857,7 +854,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="2:7" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -873,7 +870,7 @@
         <v>49</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="2:7" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -889,7 +886,7 @@
         <v>50</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="2:7" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -903,7 +900,7 @@
         <v>51</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="2:7" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -917,7 +914,7 @@
         <v>46</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -945,7 +942,7 @@
         <v>47</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -957,7 +954,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -969,7 +966,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -981,7 +978,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -993,7 +990,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>